<commit_message>
POM Framework and ExtentsReport update
</commit_message>
<xml_diff>
--- a/Selenium_Java_Tutorial_V3_141_59/src/testngsnippet/PayeeDetails.xlsx
+++ b/Selenium_Java_Tutorial_V3_141_59/src/testngsnippet/PayeeDetails.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.s\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.s\git\Selenium_Java_V19\Selenium_Java_Tutorial_V3_141_59\src\testngsnippet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -171,12 +171,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,16 +461,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="118" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" customWidth="1"/>
     <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -493,7 +495,7 @@
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">

</xml_diff>